<commit_message>
implemented tranaction and payments
</commit_message>
<xml_diff>
--- a/DataRepo/Confidential.xlsx
+++ b/DataRepo/Confidential.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebApplicationsFinalProject\client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b26f645fd8d6875/Desktop/Srikanth/Advanced Web Applications and services/Project/AdvancedWebApplication/DataRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49AFAC9-D0D2-454B-82EC-0983436CD3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{A49AFAC9-D0D2-454B-82EC-0983436CD3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB28ED70-52A6-4A27-BD3E-CF6AF87E49BA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{75F8D547-A991-4929-A79F-182D9363AE2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{75F8D547-A991-4929-A79F-182D9363AE2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Balances" sheetId="1" r:id="rId1"/>
     <sheet name="Accounts" sheetId="2" r:id="rId2"/>
-    <sheet name="UserInfo" sheetId="3" r:id="rId3"/>
+    <sheet name="AccountsInfo" sheetId="4" r:id="rId3"/>
+    <sheet name="TransactionsHistory" sheetId="5" r:id="rId4"/>
+    <sheet name="UserInfo" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>AccountName</t>
   </si>
@@ -68,19 +70,118 @@
   </si>
   <si>
     <t>Loan</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>AvailBalance</t>
+  </si>
+  <si>
+    <t>isToAccountTransferEligible</t>
+  </si>
+  <si>
+    <t>isTransferEligible</t>
+  </si>
+  <si>
+    <t>isFromAccountTransferEligible</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Mortgage</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>TransactionId</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>TransactionDate</t>
+  </si>
+  <si>
+    <t>TransactionName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>banker</t>
+  </si>
+  <si>
+    <t>a15d5e85e8</t>
+  </si>
+  <si>
+    <t>a25a2aa5566</t>
+  </si>
+  <si>
+    <t>a58d5e85d8e5</t>
+  </si>
+  <si>
+    <t>a3a255e2c24a</t>
+  </si>
+  <si>
+    <t>a8445wa5e5</t>
+  </si>
+  <si>
+    <t>MCDonalds</t>
+  </si>
+  <si>
+    <t>Purchase at mcdonalds</t>
+  </si>
+  <si>
+    <t>Broadway,Kansas</t>
+  </si>
+  <si>
+    <t>Legends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">merchandise </t>
+  </si>
+  <si>
+    <t>kansas city</t>
+  </si>
+  <si>
+    <t>merchandise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,8 +204,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,6 +224,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,20 +541,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3422462-A186-40D0-99B1-EA6FE20D62B1}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -457,10 +566,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>102548</v>
       </c>
@@ -470,11 +582,14 @@
       <c r="C2">
         <v>11111111111</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1">
+        <v>123.89</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>220055</v>
       </c>
@@ -484,11 +599,14 @@
       <c r="C3">
         <v>2222222222</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1">
+        <v>909.09</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>259862</v>
       </c>
@@ -498,8 +616,45 @@
       <c r="C4">
         <v>33333333333</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1">
+        <v>14890</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>102548</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>1234567890</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1254.02</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>102548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>1236547891</v>
+      </c>
+      <c r="D6" s="1">
+        <v>13289.9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -508,13 +663,347 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C5A504-B8FE-4599-8E0F-D187162C79FB}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF4D439-DEAB-429D-9D7B-B578456A0876}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>102548</v>
+      </c>
+      <c r="B2">
+        <v>11111111111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>102548</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>102548</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1236547891</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE118B31-A29E-42E1-B88F-0BBA1D6BF876}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>102548</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>11111111111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5.65</v>
+      </c>
+      <c r="H2" s="3">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>102548</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>1234567890</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1">
+        <v>158.21</v>
+      </c>
+      <c r="H3" s="3">
+        <v>45040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>102548</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>11111111111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="1">
+        <v>158.21</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45040</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>102548</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>11111111111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1">
+        <v>158.21</v>
+      </c>
+      <c r="H5" s="3">
+        <v>45040</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>102548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>11111111111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1">
+        <v>158.21</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45040</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C5A504-B8FE-4599-8E0F-D187162C79FB}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>102548</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>220055</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>259862</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code refactored and added some infor regarding the project
</commit_message>
<xml_diff>
--- a/DataRepo/Confidential.xlsx
+++ b/DataRepo/Confidential.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Spring 2023\AdvancedWebApplication\AdvancedWebApplication\DataRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B13F2E-F37D-4346-908D-DE3FBC7D736B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8328B8E-B5EB-46FB-97C2-00C70F7B4CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{75F8D547-A991-4929-A79F-182D9363AE2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{75F8D547-A991-4929-A79F-182D9363AE2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Balances" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="43">
   <si>
     <t>AccountName</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Checking</t>
   </si>
   <si>
-    <t>Kumar</t>
-  </si>
-  <si>
     <t>Savings</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>isFromAccountTransferEligible</t>
   </si>
   <si>
-    <t>Family</t>
-  </si>
-  <si>
     <t>Mortgage</t>
   </si>
   <si>
@@ -160,6 +154,21 @@
   </si>
   <si>
     <t>merchandise</t>
+  </si>
+  <si>
+    <t>Credit 7891</t>
+  </si>
+  <si>
+    <t>Mortgage 7890</t>
+  </si>
+  <si>
+    <t>Checking 1111</t>
+  </si>
+  <si>
+    <t>Savings 2222</t>
+  </si>
+  <si>
+    <t>Loan 3333</t>
   </si>
 </sst>
 </file>
@@ -540,12 +549,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -562,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -573,7 +582,7 @@
         <v>102548</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>11111111111</v>
@@ -590,7 +599,7 @@
         <v>220055</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>2222222222</v>
@@ -599,7 +608,7 @@
         <v>909.09</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,7 +616,7 @@
         <v>259862</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>33333333333</v>
@@ -616,7 +625,7 @@
         <v>14890</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,7 +633,7 @@
         <v>102548</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>1234567890</v>
@@ -633,7 +642,7 @@
         <v>1254.02</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,7 +650,7 @@
         <v>102548</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>1236547891</v>
@@ -650,7 +659,7 @@
         <v>13289.9</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -662,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF4D439-DEAB-429D-9D7B-B578456A0876}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +686,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -686,13 +695,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -703,7 +712,7 @@
         <v>11111111111</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -723,13 +732,13 @@
         <v>1234567890</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -743,7 +752,7 @@
         <v>1236547891</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -765,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE118B31-A29E-42E1-B88F-0BBA1D6BF876}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -781,28 +790,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -810,19 +819,19 @@
         <v>102548</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>11111111111</v>
       </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
       </c>
       <c r="G2" s="1">
         <v>5.65</v>
@@ -836,19 +845,19 @@
         <v>102548</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>1234567890</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G3" s="1">
         <v>158.21</v>
@@ -862,19 +871,19 @@
         <v>102548</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>11111111111</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1">
         <v>158.21</v>
@@ -888,19 +897,19 @@
         <v>102548</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>11111111111</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1">
         <v>158.21</v>
@@ -914,19 +923,19 @@
         <v>102548</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>11111111111</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1">
         <v>158.21</v>
@@ -940,19 +949,19 @@
         <v>102548</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>11111111111</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1">
         <v>158.21</v>
@@ -966,19 +975,19 @@
         <v>102548</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>11111111111</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8" s="1">
         <v>158.21</v>
@@ -992,19 +1001,19 @@
         <v>102548</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>11111111111</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>158.21</v>
@@ -1018,19 +1027,19 @@
         <v>102548</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>11111111111</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1">
         <v>158.21</v>
@@ -1044,19 +1053,19 @@
         <v>102548</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>11111111111</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1">
         <v>158.21</v>
@@ -1070,19 +1079,19 @@
         <v>102548</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>11111111111</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1">
         <v>158.21</v>
@@ -1096,19 +1105,19 @@
         <v>102548</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>11111111111</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G13" s="1">
         <v>158.21</v>
@@ -1122,19 +1131,19 @@
         <v>102548</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>11111111111</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G14" s="1">
         <v>158.21</v>
@@ -1148,19 +1157,19 @@
         <v>102548</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15">
         <v>11111111111</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G15" s="1">
         <v>158.21</v>
@@ -1174,19 +1183,19 @@
         <v>102548</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>11111111111</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G16" s="1">
         <v>158.21</v>
@@ -1200,19 +1209,19 @@
         <v>102548</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>11111111111</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G17" s="1">
         <v>158.21</v>
@@ -1226,19 +1235,19 @@
         <v>102548</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>11111111111</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G18" s="1">
         <v>158.21</v>
@@ -1252,19 +1261,19 @@
         <v>102548</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>11111111111</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G19" s="1">
         <v>158.21</v>
@@ -1278,19 +1287,19 @@
         <v>102548</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>11111111111</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G20" s="1">
         <v>158.21</v>
@@ -1304,19 +1313,19 @@
         <v>102548</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21">
         <v>11111111111</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G21" s="1">
         <v>158.21</v>
@@ -1330,19 +1339,19 @@
         <v>102548</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>11111111111</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G22" s="1">
         <v>158.21</v>
@@ -1356,19 +1365,19 @@
         <v>102548</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>11111111111</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G23" s="1">
         <v>158.21</v>
@@ -1382,19 +1391,19 @@
         <v>102548</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>11111111111</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G24" s="1">
         <v>158.21</v>
@@ -1408,19 +1417,19 @@
         <v>102548</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>11111111111</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G25" s="1">
         <v>158.21</v>
@@ -1434,19 +1443,19 @@
         <v>102548</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>11111111111</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G26" s="1">
         <v>158.21</v>
@@ -1460,19 +1469,19 @@
         <v>102548</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>11111111111</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G27" s="1">
         <v>158.21</v>
@@ -1486,19 +1495,19 @@
         <v>102548</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28">
         <v>11111111111</v>
       </c>
       <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" t="s">
         <v>33</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" t="s">
-        <v>35</v>
       </c>
       <c r="G28" s="1">
         <v>5.65</v>
@@ -1512,19 +1521,19 @@
         <v>102548</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29">
         <v>1234567890</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G29" s="1">
         <v>158.21</v>
@@ -1538,19 +1547,19 @@
         <v>102548</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30">
         <v>11111111111</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G30" s="1">
         <v>158.21</v>
@@ -1564,19 +1573,19 @@
         <v>102548</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31">
         <v>11111111111</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G31" s="1">
         <v>158.21</v>
@@ -1590,19 +1599,19 @@
         <v>102548</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C32">
         <v>11111111111</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G32" s="1">
         <v>158.21</v>
@@ -1616,19 +1625,19 @@
         <v>102548</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C34">
         <v>11111111111</v>
       </c>
       <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" t="s">
         <v>33</v>
-      </c>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" t="s">
-        <v>35</v>
       </c>
       <c r="G34" s="1">
         <v>5.65</v>
@@ -1642,19 +1651,19 @@
         <v>102548</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35">
         <v>1234567890</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G35" s="1">
         <v>158.21</v>
@@ -1668,19 +1677,19 @@
         <v>102548</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C36">
         <v>11111111111</v>
       </c>
       <c r="D36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G36" s="1">
         <v>158.21</v>
@@ -1694,19 +1703,19 @@
         <v>102548</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C37">
         <v>11111111111</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G37" s="1">
         <v>158.21</v>
@@ -1720,19 +1729,19 @@
         <v>102548</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C38">
         <v>11111111111</v>
       </c>
       <c r="D38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G38" s="1">
         <v>158.21</v>
@@ -1746,19 +1755,19 @@
         <v>102548</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C39">
         <v>11111111111</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G39" s="1">
         <v>158.21</v>
@@ -1772,19 +1781,19 @@
         <v>102548</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C40">
         <v>11111111111</v>
       </c>
       <c r="D40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G40" s="1">
         <v>158.21</v>
@@ -1798,19 +1807,19 @@
         <v>102548</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C41">
         <v>11111111111</v>
       </c>
       <c r="D41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F41" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G41" s="1">
         <v>158.21</v>
@@ -1824,19 +1833,19 @@
         <v>102548</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C42">
         <v>11111111111</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F42" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G42" s="1">
         <v>158.21</v>
@@ -1850,19 +1859,19 @@
         <v>102548</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C43">
         <v>11111111111</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G43" s="1">
         <v>158.21</v>
@@ -1876,19 +1885,19 @@
         <v>102548</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C44">
         <v>11111111111</v>
       </c>
       <c r="D44" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F44" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G44" s="1">
         <v>158.21</v>
@@ -1902,19 +1911,19 @@
         <v>102548</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C45">
         <v>11111111111</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G45" s="1">
         <v>158.21</v>
@@ -1928,19 +1937,19 @@
         <v>102548</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C46">
         <v>11111111111</v>
       </c>
       <c r="D46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F46" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G46" s="1">
         <v>158.21</v>
@@ -1954,19 +1963,19 @@
         <v>102548</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C47">
         <v>11111111111</v>
       </c>
       <c r="D47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E47" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F47" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G47" s="1">
         <v>158.21</v>
@@ -1980,19 +1989,19 @@
         <v>102548</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C48">
         <v>11111111111</v>
       </c>
       <c r="D48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E48" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F48" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G48" s="1">
         <v>158.21</v>
@@ -2006,19 +2015,19 @@
         <v>102548</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C49">
         <v>11111111111</v>
       </c>
       <c r="D49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G49" s="1">
         <v>158.21</v>
@@ -2032,19 +2041,19 @@
         <v>102548</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C50">
         <v>11111111111</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E50" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F50" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G50" s="1">
         <v>158.21</v>
@@ -2058,19 +2067,19 @@
         <v>102548</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C51">
         <v>11111111111</v>
       </c>
       <c r="D51" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E51" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F51" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G51" s="1">
         <v>158.21</v>
@@ -2084,19 +2093,19 @@
         <v>102548</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52">
         <v>11111111111</v>
       </c>
       <c r="D52" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F52" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G52" s="1">
         <v>158.21</v>
@@ -2110,19 +2119,19 @@
         <v>102548</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C53">
         <v>11111111111</v>
       </c>
       <c r="D53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G53" s="1">
         <v>158.21</v>
@@ -2136,19 +2145,19 @@
         <v>102548</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C54">
         <v>11111111111</v>
       </c>
       <c r="D54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F54" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G54" s="1">
         <v>158.21</v>
@@ -2162,19 +2171,19 @@
         <v>102548</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C55">
         <v>11111111111</v>
       </c>
       <c r="D55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E55" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F55" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G55" s="1">
         <v>158.21</v>
@@ -2188,19 +2197,19 @@
         <v>102548</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C56">
         <v>11111111111</v>
       </c>
       <c r="D56" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F56" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G56" s="1">
         <v>158.21</v>
@@ -2214,19 +2223,19 @@
         <v>102548</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C57">
         <v>11111111111</v>
       </c>
       <c r="D57" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E57" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F57" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G57" s="1">
         <v>158.21</v>
@@ -2240,19 +2249,19 @@
         <v>102548</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C58">
         <v>11111111111</v>
       </c>
       <c r="D58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F58" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G58" s="1">
         <v>158.21</v>
@@ -2266,19 +2275,19 @@
         <v>102548</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C59">
         <v>11111111111</v>
       </c>
       <c r="D59" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E59" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F59" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G59" s="1">
         <v>158.21</v>
@@ -2292,19 +2301,19 @@
         <v>102548</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C60">
         <v>11111111111</v>
       </c>
       <c r="D60" t="s">
+        <v>31</v>
+      </c>
+      <c r="E60" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" t="s">
         <v>33</v>
-      </c>
-      <c r="E60" t="s">
-        <v>34</v>
-      </c>
-      <c r="F60" t="s">
-        <v>35</v>
       </c>
       <c r="G60" s="1">
         <v>5.65</v>
@@ -2318,19 +2327,19 @@
         <v>102548</v>
       </c>
       <c r="B61" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C61">
         <v>1234567890</v>
       </c>
       <c r="D61" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E61" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F61" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G61" s="1">
         <v>158.21</v>
@@ -2344,19 +2353,19 @@
         <v>102548</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C62">
         <v>11111111111</v>
       </c>
       <c r="D62" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E62" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F62" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G62" s="1">
         <v>158.21</v>
@@ -2370,19 +2379,19 @@
         <v>102548</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C63">
         <v>11111111111</v>
       </c>
       <c r="D63" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E63" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F63" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G63" s="1">
         <v>158.21</v>
@@ -2396,19 +2405,19 @@
         <v>102548</v>
       </c>
       <c r="B64" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C64">
         <v>11111111111</v>
       </c>
       <c r="D64" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E64" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F64" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G64" s="1">
         <v>158.21</v>
@@ -2422,19 +2431,19 @@
         <v>102548</v>
       </c>
       <c r="B65" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C65">
         <v>11111111111</v>
       </c>
       <c r="D65" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E65" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F65" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G65" s="1">
         <v>158.21</v>
@@ -2448,19 +2457,19 @@
         <v>102548</v>
       </c>
       <c r="B66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C66">
         <v>11111111111</v>
       </c>
       <c r="D66" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E66" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F66" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G66" s="1">
         <v>158.21</v>
@@ -2474,19 +2483,19 @@
         <v>102548</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C67">
         <v>11111111111</v>
       </c>
       <c r="D67" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E67" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F67" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G67" s="1">
         <v>158.21</v>
@@ -2500,19 +2509,19 @@
         <v>102548</v>
       </c>
       <c r="B68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C68">
         <v>11111111111</v>
       </c>
       <c r="D68" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E68" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F68" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G68" s="1">
         <v>158.21</v>
@@ -2526,19 +2535,19 @@
         <v>102548</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C69">
         <v>11111111111</v>
       </c>
       <c r="D69" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E69" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F69" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G69" s="1">
         <v>158.21</v>
@@ -2552,19 +2561,19 @@
         <v>102548</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C70">
         <v>11111111111</v>
       </c>
       <c r="D70" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E70" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F70" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G70" s="1">
         <v>158.21</v>
@@ -2578,19 +2587,19 @@
         <v>102548</v>
       </c>
       <c r="B71" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C71">
         <v>11111111111</v>
       </c>
       <c r="D71" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E71" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F71" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G71" s="1">
         <v>158.21</v>
@@ -2604,19 +2613,19 @@
         <v>102548</v>
       </c>
       <c r="B72" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C72">
         <v>11111111111</v>
       </c>
       <c r="D72" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E72" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F72" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G72" s="1">
         <v>158.21</v>
@@ -2630,19 +2639,19 @@
         <v>102548</v>
       </c>
       <c r="B73" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C73">
         <v>11111111111</v>
       </c>
       <c r="D73" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E73" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F73" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G73" s="1">
         <v>158.21</v>
@@ -2656,19 +2665,19 @@
         <v>102548</v>
       </c>
       <c r="B74" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C74">
         <v>11111111111</v>
       </c>
       <c r="D74" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E74" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F74" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G74" s="1">
         <v>158.21</v>
@@ -2682,19 +2691,19 @@
         <v>102548</v>
       </c>
       <c r="B75" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C75">
         <v>11111111111</v>
       </c>
       <c r="D75" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E75" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F75" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G75" s="1">
         <v>158.21</v>
@@ -2708,19 +2717,19 @@
         <v>102548</v>
       </c>
       <c r="B76" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C76">
         <v>11111111111</v>
       </c>
       <c r="D76" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E76" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F76" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G76" s="1">
         <v>158.21</v>
@@ -2734,19 +2743,19 @@
         <v>102548</v>
       </c>
       <c r="B77" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C77">
         <v>11111111111</v>
       </c>
       <c r="D77" t="s">
+        <v>31</v>
+      </c>
+      <c r="E77" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" t="s">
         <v>33</v>
-      </c>
-      <c r="E77" t="s">
-        <v>34</v>
-      </c>
-      <c r="F77" t="s">
-        <v>35</v>
       </c>
       <c r="G77" s="1">
         <v>5.65</v>
@@ -2760,19 +2769,19 @@
         <v>102548</v>
       </c>
       <c r="B78" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C78">
         <v>1234567890</v>
       </c>
       <c r="D78" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E78" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F78" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G78" s="1">
         <v>158.21</v>
@@ -2786,19 +2795,19 @@
         <v>102548</v>
       </c>
       <c r="B79" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C79">
         <v>11111111111</v>
       </c>
       <c r="D79" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E79" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F79" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G79" s="1">
         <v>158.21</v>
@@ -2812,19 +2821,19 @@
         <v>102548</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C80">
         <v>11111111111</v>
       </c>
       <c r="D80" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E80" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F80" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G80" s="1">
         <v>158.21</v>
@@ -2838,19 +2847,19 @@
         <v>102548</v>
       </c>
       <c r="B81" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C81">
         <v>11111111111</v>
       </c>
       <c r="D81" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E81" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F81" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G81" s="1">
         <v>158.21</v>
@@ -2864,19 +2873,19 @@
         <v>102548</v>
       </c>
       <c r="B82" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C82">
         <v>11111111111</v>
       </c>
       <c r="D82" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E82" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F82" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G82" s="1">
         <v>158.21</v>
@@ -2890,19 +2899,19 @@
         <v>102548</v>
       </c>
       <c r="B83" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C83">
         <v>11111111111</v>
       </c>
       <c r="D83" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E83" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F83" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G83" s="1">
         <v>158.21</v>
@@ -2916,19 +2925,19 @@
         <v>102548</v>
       </c>
       <c r="B84" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C84">
         <v>11111111111</v>
       </c>
       <c r="D84" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E84" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F84" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G84" s="1">
         <v>158.21</v>
@@ -2942,19 +2951,19 @@
         <v>102548</v>
       </c>
       <c r="B85" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C85">
         <v>11111111111</v>
       </c>
       <c r="D85" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E85" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F85" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G85" s="1">
         <v>158.21</v>
@@ -2968,19 +2977,19 @@
         <v>102548</v>
       </c>
       <c r="B86" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C86">
         <v>11111111111</v>
       </c>
       <c r="D86" t="s">
+        <v>31</v>
+      </c>
+      <c r="E86" t="s">
+        <v>32</v>
+      </c>
+      <c r="F86" t="s">
         <v>33</v>
-      </c>
-      <c r="E86" t="s">
-        <v>34</v>
-      </c>
-      <c r="F86" t="s">
-        <v>35</v>
       </c>
       <c r="G86" s="1">
         <v>5.65</v>
@@ -2994,19 +3003,19 @@
         <v>102548</v>
       </c>
       <c r="B87" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C87">
         <v>1234567890</v>
       </c>
       <c r="D87" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E87" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F87" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G87" s="1">
         <v>158.21</v>
@@ -3020,19 +3029,19 @@
         <v>102548</v>
       </c>
       <c r="B88" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C88">
         <v>11111111111</v>
       </c>
       <c r="D88" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E88" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F88" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G88" s="1">
         <v>158.21</v>
@@ -3046,19 +3055,19 @@
         <v>102548</v>
       </c>
       <c r="B89" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C89">
         <v>11111111111</v>
       </c>
       <c r="D89" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E89" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F89" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G89" s="1">
         <v>158.21</v>
@@ -3072,19 +3081,19 @@
         <v>102548</v>
       </c>
       <c r="B90" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C90">
         <v>11111111111</v>
       </c>
       <c r="D90" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E90" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F90" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G90" s="1">
         <v>158.21</v>
@@ -3115,13 +3124,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3132,7 +3141,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3140,10 +3149,10 @@
         <v>220055</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3151,10 +3160,10 @@
         <v>259862</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>